<commit_message>
adding code to run MLP
</commit_message>
<xml_diff>
--- a/Result_data/KMeans_KNN_10.xlsx
+++ b/Result_data/KMeans_KNN_10.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="212">
   <si>
     <t>support</t>
   </si>
@@ -656,6 +656,9 @@
   </si>
   <si>
     <t>KNN Model Train Time 0.022685738589643734</t>
+  </si>
+  <si>
+    <t>f-score</t>
   </si>
 </sst>
 </file>
@@ -977,7 +980,7 @@
   <dimension ref="A1:I101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6:I96"/>
+      <selection activeCell="G11" sqref="G11:G101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1001,13 +1004,13 @@
       <c r="F1">
         <v>1</v>
       </c>
-      <c r="G1">
-        <v>1</v>
-      </c>
-      <c r="H1">
-        <v>1</v>
-      </c>
-      <c r="I1">
+      <c r="G1" t="s">
+        <v>211</v>
+      </c>
+      <c r="H1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1079,7 +1082,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1179,7 +1182,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>4</v>
       </c>
@@ -1279,7 +1282,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>4</v>
       </c>
@@ -1379,7 +1382,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>4</v>
       </c>
@@ -1479,7 +1482,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>4</v>
       </c>
@@ -1579,7 +1582,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>4</v>
       </c>
@@ -1679,7 +1682,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>4</v>
       </c>
@@ -1791,7 +1794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>4</v>
       </c>
@@ -1891,7 +1894,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>4</v>
       </c>
@@ -2003,7 +2006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>4</v>
       </c>
@@ -2103,7 +2106,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>4</v>
       </c>
@@ -2215,7 +2218,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>4</v>
       </c>
@@ -2315,7 +2318,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>4</v>
       </c>
@@ -2427,7 +2430,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>4</v>
       </c>
@@ -2536,7 +2539,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>4</v>
       </c>
@@ -2648,7 +2651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>4</v>
       </c>
@@ -2748,7 +2751,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>4</v>
       </c>
@@ -2860,7 +2863,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>4</v>
       </c>
@@ -2960,7 +2963,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>4</v>
       </c>
@@ -3072,7 +3075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>4</v>
       </c>
@@ -3105,7 +3108,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I101" xr:uid="{BD52E015-8F8D-475A-8169-CD02718186AF}">
+  <autoFilter ref="A1:I101" xr:uid="{FDF04E54-34B7-4F74-8411-25F593A97BE2}">
     <filterColumn colId="0">
       <filters>
         <filter val="4"/>
@@ -3113,7 +3116,7 @@
     </filterColumn>
     <filterColumn colId="5">
       <filters>
-        <filter val="1"/>
+        <filter val="2"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>